<commit_message>
Added new sample file
</commit_message>
<xml_diff>
--- a/assets/sample_data/sample_podata.xlsx
+++ b/assets/sample_data/sample_podata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\audit-app\assets\sample_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nilesh Gautam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="98">
   <si>
     <t>S. No.</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>14/05/2020</t>
+  </si>
+  <si>
+    <t>S. No</t>
   </si>
 </sst>
 </file>
@@ -1214,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,7 +1269,7 @@
   <sheetData>
     <row r="1" spans="1:44" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1543,7 +1546,7 @@
       <c r="W3" s="4"/>
       <c r="X3" s="4"/>
       <c r="Y3" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Z3" s="4">
         <v>10</v>
@@ -1801,7 +1804,7 @@
         <v>56</v>
       </c>
       <c r="Z6" s="4">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
@@ -1877,7 +1880,7 @@
         <v>10</v>
       </c>
       <c r="U7" s="5">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
@@ -1968,7 +1971,7 @@
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
       <c r="Y8" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Z8" s="4">
         <v>15</v>
@@ -2056,7 +2059,7 @@
         <v>56</v>
       </c>
       <c r="Z9" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AA9" s="5"/>
       <c r="AB9" s="5"/>
@@ -2132,7 +2135,7 @@
         <v>7</v>
       </c>
       <c r="U10" s="5">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>

</xml_diff>